<commit_message>
Actualizacion del diagrama de la rieda de la vida
</commit_message>
<xml_diff>
--- a/LaRuedaDeLaVida.xlsx
+++ b/LaRuedaDeLaVida.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Ciencia de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41E05DB-435B-4CCF-BB58-6FDE6A31B549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7523D4-8676-44C3-87C6-F6F8D89D012F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E116819-76AE-4011-A5D3-CF2AC795DDFB}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="LRDLV" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>Área</t>
   </si>
@@ -171,6 +170,9 @@
   <si>
     <t>Lee detenidamente cada pregunta del siguiente cuestionario. En la columna "Respuesta", marca la casilla si estás de acuerdo con la afirmación o deja el campo vacío si no aplica en tu caso.
 Este ejercicio te ayudará a evaluar diferentes aspectos de tu vida y a identificar áreas de mejora.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -285,13 +287,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -300,8 +304,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,39 +337,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-CO" b="1"/>
-              <a:t>Porcentaje de</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-CO" b="1" baseline="0"/>
-              <a:t> las areas</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-CO" b="1"/>
-              <a:t> </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -400,10 +369,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -418,16 +385,81 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>LRDLV!$F$33:$F$37</c:f>
@@ -477,7 +509,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-95C6-4C62-9D1C-58EF0B15D50D}"/>
+              <c16:uniqueId val="{00000000-EC13-4595-90BC-D05BD4F44701}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -488,119 +520,10 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="850257136"/>
-        <c:axId val="850250656"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="850257136"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="850250656"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="850250656"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="850257136"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -609,6 +532,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -687,7 +641,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -744,7 +698,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -795,6 +749,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -805,12 +766,19 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -848,7 +816,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -891,22 +859,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1011,8 +980,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1144,19 +1113,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1296,15 +1266,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>175260</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>38099</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1314,7 +1284,7 @@
                   <a14:compatExt spid="_x0000_s2049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023C254F-6515-4721-91F5-D3EEB681B01B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1360,14 +1330,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2050" name="Check Box 2" hidden="1">
@@ -1376,7 +1351,7 @@
                   <a14:compatExt spid="_x0000_s2050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B596A430-4E1F-4556-AFFB-AE6F81AB762B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1416,20 +1391,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2051" name="Check Box 3" hidden="1">
@@ -1438,7 +1418,7 @@
                   <a14:compatExt spid="_x0000_s2051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C082292A-3C57-4934-B939-31B313369AEA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1478,20 +1458,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2052" name="Check Box 4" hidden="1">
@@ -1500,7 +1485,7 @@
                   <a14:compatExt spid="_x0000_s2052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37AA7991-5D7D-4406-9026-C93AE2AA6F54}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1540,20 +1525,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2053" name="Check Box 5" hidden="1">
@@ -1562,7 +1552,7 @@
                   <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EA02D49-149C-41BD-A00A-664DA4051823}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1602,20 +1592,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>278130</xdr:colOff>
+          <xdr:colOff>281940</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2054" name="Check Box 6" hidden="1">
@@ -1624,7 +1619,7 @@
                   <a14:compatExt spid="_x0000_s2054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE916DFE-3A99-4678-AC8A-F802337891FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1664,20 +1659,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2055" name="Check Box 7" hidden="1">
@@ -1686,7 +1686,7 @@
                   <a14:compatExt spid="_x0000_s2055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6639A81-AFE7-47EC-8755-6F5EA92D7E35}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1726,20 +1726,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2056" name="Check Box 8" hidden="1">
@@ -1748,7 +1753,7 @@
                   <a14:compatExt spid="_x0000_s2056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ADAAB7A-B02E-4547-A804-79F74571999A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1788,20 +1793,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2057" name="Check Box 9" hidden="1">
@@ -1810,7 +1820,7 @@
                   <a14:compatExt spid="_x0000_s2057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8CCAA61-D46B-43D3-9166-0FFF50ECA8FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1850,20 +1860,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2058" name="Check Box 10" hidden="1">
@@ -1872,7 +1887,7 @@
                   <a14:compatExt spid="_x0000_s2058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9994DB8-6C22-4634-BF1D-1F0F449448BD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1912,20 +1927,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2059" name="Check Box 11" hidden="1">
@@ -1934,7 +1954,7 @@
                   <a14:compatExt spid="_x0000_s2059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4A568C0-AC6C-431A-A08A-EBD22E709AEA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1974,20 +1994,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2060" name="Check Box 12" hidden="1">
@@ -1996,7 +2021,7 @@
                   <a14:compatExt spid="_x0000_s2060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9E5F098-559B-4B64-AB1A-E9001B0C534E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2036,20 +2061,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>24</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2061" name="Check Box 13" hidden="1">
@@ -2058,7 +2088,7 @@
                   <a14:compatExt spid="_x0000_s2061"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C25107C4-59DE-4937-BB35-5ED6C536B29C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2098,20 +2128,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>25</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2062" name="Check Box 14" hidden="1">
@@ -2120,7 +2155,7 @@
                   <a14:compatExt spid="_x0000_s2062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20B70BED-0BEC-4B03-8AE3-C65E3AD18102}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2160,20 +2195,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2063" name="Check Box 15" hidden="1">
@@ -2182,7 +2222,7 @@
                   <a14:compatExt spid="_x0000_s2063"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69D914AA-A0A2-4DE7-83C4-D3E6F311BC33}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2222,20 +2262,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2064" name="Check Box 16" hidden="1">
@@ -2244,7 +2289,7 @@
                   <a14:compatExt spid="_x0000_s2064"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACC46E75-4D6E-4754-9328-CDBDAAC86742}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2284,20 +2329,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2065" name="Check Box 17" hidden="1">
@@ -2306,7 +2356,7 @@
                   <a14:compatExt spid="_x0000_s2065"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FE07B9B-D38E-4083-ABE4-DBD58DB25119}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2346,20 +2396,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2066" name="Check Box 18" hidden="1">
@@ -2368,7 +2423,7 @@
                   <a14:compatExt spid="_x0000_s2066"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DBAF84C-3750-46EC-ADE7-7EE6503E5DBD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2408,20 +2463,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2067" name="Check Box 19" hidden="1">
@@ -2430,7 +2490,7 @@
                   <a14:compatExt spid="_x0000_s2067"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75990E85-5256-431E-8D00-9B316ABF3B34}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2470,20 +2530,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2068" name="Check Box 20" hidden="1">
@@ -2492,7 +2557,7 @@
                   <a14:compatExt spid="_x0000_s2068"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CDB6599-EC11-4ABB-832A-007C69C47EB5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2532,20 +2597,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2069" name="Check Box 21" hidden="1">
@@ -2554,7 +2624,7 @@
                   <a14:compatExt spid="_x0000_s2069"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A3AA17-75B0-4E42-945C-8AFB73352F4A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2594,20 +2664,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2070" name="Check Box 22" hidden="1">
@@ -2616,7 +2691,7 @@
                   <a14:compatExt spid="_x0000_s2070"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8746956B-07FF-469C-AC88-561E004B9E42}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2656,20 +2731,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2071" name="Check Box 23" hidden="1">
@@ -2678,7 +2758,7 @@
                   <a14:compatExt spid="_x0000_s2071"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{755FAE52-4B37-4C46-B0D7-3F0D9D36CF42}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2718,20 +2798,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="680085" cy="247650"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2072" name="Check Box 24" hidden="1">
@@ -2740,7 +2825,7 @@
                   <a14:compatExt spid="_x0000_s2072"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAF8D280-3C57-4DE1-9C28-08F3880B386A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2780,20 +2865,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683895" cy="247650"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>175260</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2073" name="Check Box 25" hidden="1">
@@ -2802,7 +2892,7 @@
                   <a14:compatExt spid="_x0000_s2073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03B781B7-E1A7-4AF1-8EB0-2070329D12C3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2842,29 +2932,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>113306</xdr:colOff>
+      <xdr:colOff>207065</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>130700</xdr:rowOff>
+      <xdr:rowOff>86140</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>710647</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>130700</xdr:rowOff>
+      <xdr:rowOff>96079</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4033DB00-200B-0C95-EB58-28963E7DD1AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAE8BBA8-7D89-B9D0-68A5-53885B1CD461}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3202,10 +3292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA42CD9-354B-4C7C-A678-981821A6BB9E}">
-  <dimension ref="B1:H37"/>
+  <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3218,44 +3308,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
@@ -3278,102 +3368,102 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="10" t="b">
+      <c r="D8" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="10" t="b">
+      <c r="H8" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="10" t="b">
+      <c r="D9" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="10" t="b">
+      <c r="H9" s="7" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="10" t="b">
+      <c r="D10" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="10" t="b">
+      <c r="H10" s="7" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="10" t="b">
+      <c r="D11" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="10" t="b">
+      <c r="H11" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="10" t="b">
+      <c r="D12" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="10" t="b">
+      <c r="H12" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3398,102 +3488,102 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="10" t="b">
+      <c r="D16" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="10" t="b">
+      <c r="H16" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="10" t="b">
+      <c r="D17" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="10" t="b">
+      <c r="H17" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="10" t="b">
+      <c r="D18" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="10" t="b">
+      <c r="H18" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="10" t="b">
+      <c r="D19" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="10" t="b">
+      <c r="H19" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="10" t="b">
+      <c r="D20" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="10" t="b">
+      <c r="H20" s="7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3509,65 +3599,65 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="10" t="b">
+      <c r="D24" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="10" t="b">
+      <c r="D25" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="10" t="b">
+      <c r="D26" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="10" t="b">
+      <c r="D27" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="10" t="b">
+      <c r="D28" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3575,7 +3665,7 @@
       <c r="F33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G33" s="6" cm="1">
+      <c r="G33" s="5" cm="1">
         <f t="array" ref="G33">AVERAGE(--D8:D12)</f>
         <v>0.6</v>
       </c>
@@ -3584,7 +3674,7 @@
       <c r="F34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="6" cm="1">
+      <c r="G34" s="5" cm="1">
         <f t="array" ref="G34">AVERAGE(--D16:D20)</f>
         <v>1</v>
       </c>
@@ -3593,7 +3683,7 @@
       <c r="F35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G35" s="6" cm="1">
+      <c r="G35" s="5" cm="1">
         <f t="array" ref="G35">AVERAGE(--D24:D28)</f>
         <v>1</v>
       </c>
@@ -3602,7 +3692,7 @@
       <c r="F36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="6" cm="1">
+      <c r="G36" s="5" cm="1">
         <f t="array" ref="G36">AVERAGE(--H8:H12)</f>
         <v>0.4</v>
       </c>
@@ -3611,9 +3701,14 @@
       <c r="F37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="6" cm="1">
+      <c r="G37" s="5" cm="1">
         <f t="array" ref="G37">AVERAGE(--H16:H20)</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>